<commit_message>
Update balans file and change message language
</commit_message>
<xml_diff>
--- a/Teoria/Balans.xlsx
+++ b/Teoria/Balans.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Balans" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
   <si>
     <t>Minimalna liczba kostek</t>
   </si>
@@ -51,6 +51,69 @@
   </si>
   <si>
     <t>Wartość cechy</t>
+  </si>
+  <si>
+    <t>Minimalna wartość zdrowia</t>
+  </si>
+  <si>
+    <t>Maksymalna wartość zdrowia</t>
+  </si>
+  <si>
+    <t>Liczba członków drużyny</t>
+  </si>
+  <si>
+    <t>Maksymalna wartość zdrowia Startowa</t>
+  </si>
+  <si>
+    <t>Wynik kości</t>
+  </si>
+  <si>
+    <t>Wartość</t>
+  </si>
+  <si>
+    <t>Wzór</t>
+  </si>
+  <si>
+    <t>Wartość oczekiwana</t>
+  </si>
+  <si>
+    <t>Suma</t>
+  </si>
+  <si>
+    <t>Miecz</t>
+  </si>
+  <si>
+    <t>Liczba kości</t>
+  </si>
+  <si>
+    <t>Odchylenie</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1x dmg</t>
+  </si>
+  <si>
+    <t>Topór</t>
+  </si>
+  <si>
+    <t>2x dmg</t>
+  </si>
+  <si>
+    <t>Łuk</t>
+  </si>
+  <si>
+    <t>Sztylet</t>
+  </si>
+  <si>
+    <t>0.5x dmg</t>
+  </si>
+  <si>
+    <t>2.5x dmg</t>
+  </si>
+  <si>
+    <t>1.5x dmg</t>
   </si>
 </sst>
 </file>
@@ -58,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -77,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -85,11 +148,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -97,7 +309,55 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -401,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +688,7 @@
       </c>
       <c r="D1" s="3">
         <f>B5*B4*(1+B6)*B7</f>
-        <v>15.600000000000001</v>
+        <v>31.200000000000003</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -449,14 +709,14 @@
       </c>
       <c r="D2" s="3">
         <f>ROUND(D1+B9,0)</f>
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1">
         <v>3</v>
       </c>
       <c r="F2" s="2">
-        <f>$B$8+($D$2-$B$8)/($B$2-$B$1)*(E2-$B$1)</f>
-        <v>6</v>
+        <f>ROUND($B$8+($D$2-$B$8)/($B$2-$B$1)*(E2-$B$1),0)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -466,12 +726,19 @@
       <c r="B3" s="3">
         <v>4</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <f>B10*B8</f>
+        <v>36</v>
+      </c>
       <c r="E3" s="1">
         <v>4</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F9" si="0">$B$8+($D$2-$B$8)/($B$2-$B$1)*(E3-$B$1)</f>
-        <v>9.1428571428571423</v>
+        <f t="shared" ref="F3:F9" si="0">ROUND($B$8+($D$2-$B$8)/($B$2-$B$1)*(E3-$B$1),0)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -481,27 +748,41 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <f>B10*D2</f>
+        <v>165</v>
+      </c>
       <c r="E4" s="1">
         <v>5</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>12.285714285714285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <f>B10*B9</f>
+        <v>72</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>15.428571428571429</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,7 +797,7 @@
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>18.571428571428569</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -531,7 +812,7 @@
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>21.714285714285715</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -539,14 +820,14 @@
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1">
         <v>9</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>24.857142857142858</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,14 +835,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -571,17 +860,688 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="25" width="12.7109375" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="E1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="I1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="M1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="13">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="14">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="14">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="14">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4">
+        <v>2</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="14">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="14">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="14">
+        <v>3</v>
+      </c>
+      <c r="N5" s="4">
+        <v>2</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="14">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="14">
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <v>3</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="14">
+        <v>4</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="14">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="14">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>7</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="14">
+        <v>5</v>
+      </c>
+      <c r="N7" s="4">
+        <v>4</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="15">
+        <v>6</v>
+      </c>
+      <c r="F8" s="11">
+        <v>10</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="15">
+        <v>6</v>
+      </c>
+      <c r="J8" s="11">
+        <v>7</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="15">
+        <v>6</v>
+      </c>
+      <c r="N8" s="11">
+        <v>10</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="8">
+        <f>SUM(B3:B8)/6</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="8">
+        <f>SUM(F3:F8)/6</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="8">
+        <f>SUM(J3:J8)/6</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="8">
+        <f>SUM(N3:N8)/6</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="9">
+        <f>_xlfn.STDEV.P(B3:B8)</f>
+        <v>2.4944382578492941</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9">
+        <f>_xlfn.STDEV.P(F3:F8)</f>
+        <v>3.7267799624996494</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="9">
+        <f>_xlfn.STDEV.P(J3:J8)</f>
+        <v>2.8674417556808756</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="9">
+        <f>_xlfn.STDEV.P(N3:N8)</f>
+        <v>3.197221015541813</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="12">
+        <f>SUM(B3:B8)</f>
+        <v>20</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="12">
+        <f>SUM(F3:F8)</f>
+        <v>20</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="12">
+        <f>SUM(J3:J8)</f>
+        <v>20</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="12">
+        <f>SUM(N3:N8)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <f>A16*$B$10</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="C16" s="9">
+        <f>SQRT(A16)*$B$11</f>
+        <v>3.5276684147527875</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="9">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*$F$10</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="G16" s="9">
+        <f>SQRT(E16)*$F$11</f>
+        <v>5.2704627669472988</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="9">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1">
+        <f>I16*$J$10</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="K16" s="9">
+        <f>SQRT(I16)*$J$11</f>
+        <v>4.0551750201988135</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="9">
+        <v>2</v>
+      </c>
+      <c r="N16" s="1">
+        <f>M16*$N$10</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="O16" s="9">
+        <f>SQRT(M16)*$N$11</f>
+        <v>4.5215533220835127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <f>A17*$B$10</f>
+        <v>10</v>
+      </c>
+      <c r="C17" s="9">
+        <f>SQRT(A17)*$B$11</f>
+        <v>4.320493798938573</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="9">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17:F20" si="0">E17*$F$10</f>
+        <v>10</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" ref="G17:G20" si="1">SQRT(E17)*$F$11</f>
+        <v>6.4549722436790278</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="9">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" ref="J17:J20" si="2">I17*$J$10</f>
+        <v>10</v>
+      </c>
+      <c r="K17" s="9">
+        <f t="shared" ref="K17:K20" si="3">SQRT(I17)*$J$11</f>
+        <v>4.9665548085837798</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="9">
+        <v>3</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" ref="N17:N20" si="4">M17*$N$10</f>
+        <v>10</v>
+      </c>
+      <c r="O17" s="9">
+        <f t="shared" ref="O17:O20" si="5">SQRT(M17)*$N$11</f>
+        <v>5.5377492419453826</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" ref="B18:B20" si="6">A18*$B$10</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" ref="C18:C20" si="7">SQRT(A18)*$B$11</f>
+        <v>4.9888765156985881</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="9">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>7.4535599249992988</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="9">
+        <v>4</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="K18" s="9">
+        <f t="shared" si="3"/>
+        <v>5.7348835113617511</v>
+      </c>
+      <c r="L18" s="14"/>
+      <c r="M18" s="9">
+        <v>4</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="4"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="O18" s="9">
+        <f t="shared" si="5"/>
+        <v>6.3944420310836261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="6"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="7"/>
+        <v>5.5777335102271701</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="9">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="9">
+        <v>5</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K19" s="9">
+        <f t="shared" si="3"/>
+        <v>6.4117946872237814</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="9">
+        <v>5</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="4"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="O19" s="9">
+        <f t="shared" si="5"/>
+        <v>7.1492035298424055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>6</v>
+      </c>
+      <c r="B20" s="10">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="7"/>
+        <v>6.1101009266077853</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="12">
+        <v>6</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="1"/>
+        <v>9.1287092917527684</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="12">
+        <v>6</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="K20" s="12">
+        <f t="shared" si="3"/>
+        <v>7.0237691685684922</v>
+      </c>
+      <c r="L20" s="14"/>
+      <c r="M20" s="12">
+        <v>6</v>
+      </c>
+      <c r="N20" s="10">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="O20" s="12">
+        <f t="shared" si="5"/>
+        <v>7.8315600829804861</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix bugs in DiceItemGenerator
</commit_message>
<xml_diff>
--- a/Teoria/Balans.xlsx
+++ b/Teoria/Balans.xlsx
@@ -370,6 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -379,7 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -684,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
     <col min="5" max="6" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -734,21 +734,21 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>ROUND(D1+B9,0)</f>
-        <v>161</v>
+        <f>ROUND(D1+B8,0)</f>
+        <v>139</v>
       </c>
       <c r="E2" s="1">
         <v>3</v>
       </c>
       <c r="F2" s="2">
         <f>ROUND($B$8+($D$2-$B$8)/($B$2-$B$1)*(E2-$B$1),0)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -760,21 +760,21 @@
       </c>
       <c r="D3" s="3">
         <f>B10*B8</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F9" si="0">ROUND($B$8+($D$2-$B$8)/($B$2-$B$1)*(E3-$B$1),0)</f>
-        <v>33</v>
-      </c>
-      <c r="G3" s="19">
+        <v>32</v>
+      </c>
+      <c r="G3" s="16">
         <f>F3-F2</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -786,21 +786,21 @@
       </c>
       <c r="D4" s="3">
         <f>B10*D2</f>
-        <v>483</v>
+        <v>417</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="G4" s="19">
+        <v>50</v>
+      </c>
+      <c r="G4" s="16">
         <f t="shared" ref="G4:G9" si="1">F4-F3</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -812,21 +812,21 @@
       </c>
       <c r="D5" s="3">
         <f>B10*B9</f>
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="G5" s="19">
+        <v>68</v>
+      </c>
+      <c r="G5" s="16">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -838,14 +838,14 @@
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="G6" s="19">
+        <v>85</v>
+      </c>
+      <c r="G6" s="16">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -857,60 +857,82 @@
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="G7" s="19">
+        <v>103</v>
+      </c>
+      <c r="G7" s="16">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>9</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="G8" s="19">
+        <v>121</v>
+      </c>
+      <c r="G8" s="16">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>36</v>
+        <f>F4</f>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>161</v>
-      </c>
-      <c r="G9" s="19">
+        <v>139</v>
+      </c>
+      <c r="G9" s="16">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="H9">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:F11" si="2">ROUND($B$8+($D$2-$B$8)/($B$2-$B$1)*(E10-$B$1),0)</f>
+        <v>157</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" ref="G10:G11" si="3">F10-F9</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -932,36 +954,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
-      <c r="I1" s="16" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="I1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="M1" s="16" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="M1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="18"/>
-      <c r="Q1" s="16" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="19"/>
+      <c r="Q1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="17"/>
-      <c r="S1" s="18"/>
-      <c r="U1" s="16" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="19"/>
+      <c r="U1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="17"/>
-      <c r="W1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">

</xml_diff>

<commit_message>
Add more enemy base
</commit_message>
<xml_diff>
--- a/Teoria/Balans.xlsx
+++ b/Teoria/Balans.xlsx
@@ -4,15 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Gracz" sheetId="1" r:id="rId1"/>
     <sheet name="Akcje" sheetId="5" r:id="rId2"/>
     <sheet name="Przedmioty" sheetId="6" r:id="rId3"/>
     <sheet name="Zaklęcia" sheetId="8" r:id="rId4"/>
+    <sheet name="Przeciwnicy" sheetId="9" r:id="rId5"/>
+    <sheet name="Akcje przeciwników" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="113">
   <si>
     <t>Minimalna liczba kostek</t>
   </si>
@@ -249,6 +252,126 @@
   </si>
   <si>
     <t>ghost sword</t>
+  </si>
+  <si>
+    <t>Min. Cechy</t>
+  </si>
+  <si>
+    <t>Maks. Cechy</t>
+  </si>
+  <si>
+    <t>Cechy</t>
+  </si>
+  <si>
+    <t>Kategorię</t>
+  </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>Minion</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>HP mod</t>
+  </si>
+  <si>
+    <t>Wartość</t>
+  </si>
+  <si>
+    <t>Min. Dodatkowe bonusy</t>
+  </si>
+  <si>
+    <t>Mod. akcji</t>
+  </si>
+  <si>
+    <t>Przykładowe HP</t>
+  </si>
+  <si>
+    <t>Siła</t>
+  </si>
+  <si>
+    <t>Efekt</t>
+  </si>
+  <si>
+    <t>weakAttack</t>
+  </si>
+  <si>
+    <t>attack</t>
+  </si>
+  <si>
+    <t>veryWeak</t>
+  </si>
+  <si>
+    <t>weak</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>veryStrong</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>strongAttack</t>
+  </si>
+  <si>
+    <t>deadlyAttack</t>
+  </si>
+  <si>
+    <t>defence</t>
+  </si>
+  <si>
+    <t>invinclibleDefence</t>
+  </si>
+  <si>
+    <t>weakRegen</t>
+  </si>
+  <si>
+    <t>Regen</t>
+  </si>
+  <si>
+    <t>goodRegen</t>
+  </si>
+  <si>
+    <t>poison</t>
+  </si>
+  <si>
+    <t>deadlyPoison</t>
+  </si>
+  <si>
+    <t>bleed</t>
+  </si>
+  <si>
+    <t>strongBleed</t>
+  </si>
+  <si>
+    <t>weakness</t>
+  </si>
+  <si>
+    <t>deadlyWeakness</t>
+  </si>
+  <si>
+    <t>strongWeakness</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>weakCounter</t>
+  </si>
+  <si>
+    <t>goodCounter</t>
+  </si>
+  <si>
+    <t>badDefence</t>
+  </si>
+  <si>
+    <t>nieużywane</t>
   </si>
 </sst>
 </file>
@@ -284,7 +407,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -292,11 +415,147 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -325,10 +584,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -654,23 +989,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="22"/>
+      <c r="D1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="J1" s="9" t="s">
+      <c r="H1" s="23"/>
+      <c r="J1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -924,7 +1259,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1366,7 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,14 +1389,14 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -1840,7 +2175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1856,14 +2191,14 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
@@ -2233,4 +2568,1023 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="11.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
+    <col min="5" max="7" width="10.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="4">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="4">
+        <v>100</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K4" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="27"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="12">
+        <v>10</v>
+      </c>
+      <c r="L5" s="13">
+        <v>30</v>
+      </c>
+      <c r="M5" s="13">
+        <v>50</v>
+      </c>
+      <c r="N5" s="13">
+        <v>70</v>
+      </c>
+      <c r="O5" s="14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="15">
+        <f>K$5*$E$2</f>
+        <v>10</v>
+      </c>
+      <c r="L6" s="16">
+        <f t="shared" ref="L6:O6" si="0">L$5*$E$2</f>
+        <v>30</v>
+      </c>
+      <c r="M6" s="16">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N6" s="16">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="O6" s="17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" s="15">
+        <f>K$5*$F$2</f>
+        <v>30</v>
+      </c>
+      <c r="L7" s="16">
+        <f t="shared" ref="L7:O7" si="1">L$5*$F$2</f>
+        <v>90</v>
+      </c>
+      <c r="M7" s="16">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="N7" s="16">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="O7" s="17">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="18">
+        <f>K$5*$G$2</f>
+        <v>50</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" ref="L8:O8" si="2">L$5*$G$2</f>
+        <v>150</v>
+      </c>
+      <c r="M8" s="10">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="2"/>
+        <v>350</v>
+      </c>
+      <c r="O8" s="11">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K4:O4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="28" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="7" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="32">
+        <v>10</v>
+      </c>
+      <c r="E2" s="33">
+        <v>30</v>
+      </c>
+      <c r="F2" s="33">
+        <v>50</v>
+      </c>
+      <c r="G2" s="33">
+        <v>75</v>
+      </c>
+      <c r="H2" s="34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="29">
+        <f>D$2*VLOOKUP($C3,Przeciwnicy!$A$5:$B$10,2)/VLOOKUP($B3,Akcje!$A$1:$B$11,2)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="29">
+        <f>E$2*VLOOKUP($C3,Przeciwnicy!$A$5:$B$10,2)/VLOOKUP($B3,Akcje!$A$1:$B$11,2)</f>
+        <v>6</v>
+      </c>
+      <c r="F3" s="29">
+        <f>F$2*VLOOKUP($C3,Przeciwnicy!$A$5:$B$10,2)/VLOOKUP($B3,Akcje!$A$1:$B$11,2)</f>
+        <v>10</v>
+      </c>
+      <c r="G3" s="29">
+        <f>G$2*VLOOKUP($C3,Przeciwnicy!$A$5:$B$10,2)/VLOOKUP($B3,Akcje!$A$1:$B$11,2)</f>
+        <v>15</v>
+      </c>
+      <c r="H3" s="35">
+        <f>H$2*VLOOKUP($C3,Przeciwnicy!$A$5:$B$10,2)/VLOOKUP($B3,Akcje!$A$1:$B$11,2)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="29">
+        <f>D$2*VLOOKUP($C4,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B4,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="29">
+        <f>E$2*VLOOKUP($C4,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B4,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="F4" s="29">
+        <f>F$2*VLOOKUP($C4,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B4,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="G4" s="29">
+        <f>G$2*VLOOKUP($C4,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B4,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>22.5</v>
+      </c>
+      <c r="H4" s="36">
+        <f>H$2*VLOOKUP($C4,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B4,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="29">
+        <f>D$2*VLOOKUP($C5,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B5,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="E5" s="29">
+        <f>E$2*VLOOKUP($C5,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B5,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F5" s="29">
+        <f>F$2*VLOOKUP($C5,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B5,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="G5" s="29">
+        <f>G$2*VLOOKUP($C5,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B5,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>37.5</v>
+      </c>
+      <c r="H5" s="36">
+        <f>H$2*VLOOKUP($C5,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B5,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="29">
+        <f>D$2*VLOOKUP($C6,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B6,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="E6" s="29">
+        <f>E$2*VLOOKUP($C6,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B6,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="F6" s="29">
+        <f>F$2*VLOOKUP($C6,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B6,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="G6" s="29">
+        <f>G$2*VLOOKUP($C6,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B6,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>52.5</v>
+      </c>
+      <c r="H6" s="36">
+        <f>H$2*VLOOKUP($C6,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B6,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="29">
+        <f>D$2*VLOOKUP($C7,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B7,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="29">
+        <f>E$2*VLOOKUP($C7,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B7,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="29">
+        <f>F$2*VLOOKUP($C7,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B7,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="G7" s="29">
+        <f>G$2*VLOOKUP($C7,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B7,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>22.5</v>
+      </c>
+      <c r="H7" s="36">
+        <f>H$2*VLOOKUP($C7,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B7,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="29">
+        <f>D$2*VLOOKUP($C8,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B8,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="E8" s="29">
+        <f>E$2*VLOOKUP($C8,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B8,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="F8" s="29">
+        <f>F$2*VLOOKUP($C8,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B8,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="G8" s="29">
+        <f>G$2*VLOOKUP($C8,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B8,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>52.5</v>
+      </c>
+      <c r="H8" s="36">
+        <f>H$2*VLOOKUP($C8,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B8,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="29">
+        <f>D$2*VLOOKUP($C9,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B9,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="29">
+        <f>E$2*VLOOKUP($C9,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B9,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="29">
+        <f>F$2*VLOOKUP($C9,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B9,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="29">
+        <f>G$2*VLOOKUP($C9,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B9,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H9" s="36">
+        <f>H$2*VLOOKUP($C9,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B9,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="29">
+        <f>D$2*VLOOKUP($C10,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B10,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="29">
+        <f>E$2*VLOOKUP($C10,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B10,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="29">
+        <f>F$2*VLOOKUP($C10,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B10,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="G10" s="29">
+        <f>G$2*VLOOKUP($C10,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B10,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>11.25</v>
+      </c>
+      <c r="H10" s="36">
+        <f>H$2*VLOOKUP($C10,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B10,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="29">
+        <f>D$2*VLOOKUP($C11,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B11,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="29">
+        <f>E$2*VLOOKUP($C11,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B11,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="F11" s="29">
+        <f>F$2*VLOOKUP($C11,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B11,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>12.5</v>
+      </c>
+      <c r="G11" s="29">
+        <f>G$2*VLOOKUP($C11,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B11,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>18.75</v>
+      </c>
+      <c r="H11" s="36">
+        <f>H$2*VLOOKUP($C11,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B11,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="29">
+        <f>D$2*VLOOKUP($C12,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B12,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="29">
+        <f>E$2*VLOOKUP($C12,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B12,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F12" s="29">
+        <f>F$2*VLOOKUP($C12,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B12,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="G12" s="29">
+        <f>G$2*VLOOKUP($C12,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B12,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H12" s="36">
+        <f>H$2*VLOOKUP($C12,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B12,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="29">
+        <f>D$2*VLOOKUP($C13,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B13,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="E13" s="29">
+        <f>E$2*VLOOKUP($C13,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B13,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="F13" s="29">
+        <f>F$2*VLOOKUP($C13,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B13,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="G13" s="29">
+        <f>G$2*VLOOKUP($C13,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B13,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>17.5</v>
+      </c>
+      <c r="H13" s="36">
+        <f>H$2*VLOOKUP($C13,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B13,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>23.333333333333332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="29">
+        <f>D$2*VLOOKUP($C14,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B14,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="29">
+        <f>E$2*VLOOKUP($C14,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B14,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1.8</v>
+      </c>
+      <c r="F14" s="29">
+        <f>F$2*VLOOKUP($C14,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B14,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G14" s="29">
+        <f>G$2*VLOOKUP($C14,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B14,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>4.5</v>
+      </c>
+      <c r="H14" s="36">
+        <f>H$2*VLOOKUP($C14,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B14,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="29">
+        <f>D$2*VLOOKUP($C15,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B15,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="29">
+        <f>E$2*VLOOKUP($C15,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B15,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F15" s="29">
+        <f>F$2*VLOOKUP($C15,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B15,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="29">
+        <f>G$2*VLOOKUP($C15,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B15,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H15" s="36">
+        <f>H$2*VLOOKUP($C15,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B15,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="29">
+        <f>D$2*VLOOKUP($C16,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B16,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E16" s="29">
+        <f>E$2*VLOOKUP($C16,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B16,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>2.25</v>
+      </c>
+      <c r="F16" s="29">
+        <f>F$2*VLOOKUP($C16,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B16,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3.75</v>
+      </c>
+      <c r="G16" s="29">
+        <f>G$2*VLOOKUP($C16,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B16,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5.625</v>
+      </c>
+      <c r="H16" s="36">
+        <f>H$2*VLOOKUP($C16,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B16,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="29">
+        <f>D$2*VLOOKUP($C17,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B17,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1.75</v>
+      </c>
+      <c r="E17" s="29">
+        <f>E$2*VLOOKUP($C17,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B17,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5.25</v>
+      </c>
+      <c r="F17" s="29">
+        <f>F$2*VLOOKUP($C17,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B17,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>8.75</v>
+      </c>
+      <c r="G17" s="29">
+        <f>G$2*VLOOKUP($C17,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B17,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>13.125</v>
+      </c>
+      <c r="H17" s="36">
+        <f>H$2*VLOOKUP($C17,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B17,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="29">
+        <f>D$2*VLOOKUP($C18,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B18,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E18" s="29">
+        <f>E$2*VLOOKUP($C18,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B18,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3.75</v>
+      </c>
+      <c r="F18" s="29">
+        <f>F$2*VLOOKUP($C18,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B18,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>6.25</v>
+      </c>
+      <c r="G18" s="29">
+        <f>G$2*VLOOKUP($C18,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B18,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>9.375</v>
+      </c>
+      <c r="H18" s="36">
+        <f>H$2*VLOOKUP($C18,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B18,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="29">
+        <f>D$2*VLOOKUP($C19,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B19,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="29">
+        <f>E$2*VLOOKUP($C19,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B19,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>4.5</v>
+      </c>
+      <c r="F19" s="29">
+        <f>F$2*VLOOKUP($C19,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B19,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="G19" s="29">
+        <f>G$2*VLOOKUP($C19,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B19,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>11.25</v>
+      </c>
+      <c r="H19" s="36">
+        <f>H$2*VLOOKUP($C19,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B19,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="29">
+        <f>D$2*VLOOKUP($C20,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B20,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="29">
+        <f>E$2*VLOOKUP($C20,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B20,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="29">
+        <f>F$2*VLOOKUP($C20,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B20,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="29">
+        <f>G$2*VLOOKUP($C20,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B20,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H20" s="36">
+        <f>H$2*VLOOKUP($C20,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B20,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="29">
+        <f>D$2*VLOOKUP($C21,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B21,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="29">
+        <f>E$2*VLOOKUP($C21,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B21,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>7.5</v>
+      </c>
+      <c r="F21" s="29">
+        <f>F$2*VLOOKUP($C21,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B21,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>12.5</v>
+      </c>
+      <c r="G21" s="29">
+        <f>G$2*VLOOKUP($C21,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B21,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>18.75</v>
+      </c>
+      <c r="H21" s="36">
+        <f>H$2*VLOOKUP($C21,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B21,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="29">
+        <f>D$2*VLOOKUP($C22,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B22,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E22" s="29">
+        <f>E$2*VLOOKUP($C22,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B22,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="F22" s="29">
+        <f>F$2*VLOOKUP($C22,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B22,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="G22" s="29">
+        <f>G$2*VLOOKUP($C22,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B22,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="H22" s="36">
+        <f>H$2*VLOOKUP($C22,Przeciwnicy!$A$6:$B$10,2,FALSE)/VLOOKUP($B22,Akcje!$A$1:$B$11,2,FALSE)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+      <c r="H23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="42"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="42"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="42"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="42"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="42"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="42"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>